<commit_message>
use of the new code
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{602BBAFE-1B25-42F0-B2CD-967C635A7E21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{52259953-7160-4941-8869-C4CA6A270375}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BEDD22B4-E9A7-41DE-A77C-291F23F69BD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BEDD22B4-E9A7-41DE-A77C-291F23F69BD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -784,12 +784,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -801,6 +795,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1062,14 +1062,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C2190243-D331-4AFC-BE0E-97FD26C4A11A}" name="Table3" displayName="Table3" ref="A1:E3" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C2190243-D331-4AFC-BE0E-97FD26C4A11A}" name="Table3" displayName="Table3" ref="A1:E3" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E3" xr:uid="{AB15CA78-7031-4CCA-B9A0-F71CC4EE9A5E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{14A87E81-A21B-42A7-9C51-165EDBE75BD2}" name="日期" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{FABE051F-B3F5-4E93-B893-6AE31602B978}" name="版本" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{CDA8112A-005D-44F5-AD43-31F9E9476FBE}" name="更新內容" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{9F516A1A-B600-47B5-ACF2-AC59149C316A}" name="新增造字" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{18F22CDC-7F06-4D68-BE8B-76A838841B87}" name="備註" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{14A87E81-A21B-42A7-9C51-165EDBE75BD2}" name="日期" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{FABE051F-B3F5-4E93-B893-6AE31602B978}" name="版本" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{CDA8112A-005D-44F5-AD43-31F9E9476FBE}" name="更新內容" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9F516A1A-B600-47B5-ACF2-AC59149C316A}" name="新增造字" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{18F22CDC-7F06-4D68-BE8B-76A838841B87}" name="備註" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1375,7 +1375,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1523,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4D26C7-4F65-403D-902E-42EDF5FC54F2}">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -2387,7 +2387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFEA6B0-793C-4098-A023-30FD6B6C6D7D}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>